<commit_message>
add free shipping field
</commit_message>
<xml_diff>
--- a/public/backend/media/shipping_bulk_import.xlsx
+++ b/public/backend/media/shipping_bulk_import.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arsalan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\epcafe\public\backend\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A05ABBF-120B-496E-B5D3-97597EDC2E10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C23CC3-7ABD-44B2-87D2-487B19F6A0D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ListMonths">OFFSET(Sheet1!$C$1,1,0,MAX(Sheet1!$A:$A),1)</definedName>
+    <definedName name="ListMonths">OFFSET(Sheet1!$D$1,1,0,MAX(Sheet1!$A:$A),1)</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Pincode</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>Inactive</t>
+  </si>
+  <si>
+    <t>Free Shipping</t>
   </si>
 </sst>
 </file>
@@ -444,89 +447,97 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17" style="4" customWidth="1"/>
-    <col min="2" max="2" width="14" style="4" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="17" style="4" customWidth="1"/>
+    <col min="3" max="3" width="14" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>282007</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3">
         <v>20</v>
       </c>
-      <c r="C2" s="3">
+      <c r="D2" s="3">
         <v>10</v>
       </c>
-      <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="3"/>
+      <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>282003</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3">
         <v>10</v>
       </c>
-      <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="3"/>
+      <c r="G3" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>282005</v>
       </c>
       <c r="B4" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C4" s="3">
         <v>200</v>
       </c>
-      <c r="C4" s="3">
+      <c r="D4" s="3">
         <v>300</v>
       </c>
-      <c r="D4" s="3">
+      <c r="E4" s="3">
         <v>400</v>
       </c>
-      <c r="E4" s="3">
+      <c r="F4" s="3">
         <v>500</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>